<commit_message>
+ Modify user interface
</commit_message>
<xml_diff>
--- a/OJT/Upload/Template/Export/OJT_EXP1.xlsx
+++ b/OJT/Upload/Template/Export/OJT_EXP1.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20304"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20314"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0ACAB824-031F-4E95-B96A-519C14665DB7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8B86AD6-7DC0-444E-B261-9ACD97DA8968}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>EM ID</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Score</t>
+  </si>
+  <si>
+    <t>Archievement</t>
   </si>
 </sst>
 </file>
@@ -95,7 +98,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -144,21 +147,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -475,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:R4"/>
+  <dimension ref="B2:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="P2" sqref="P2:S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -498,94 +547,98 @@
     <col min="14" max="14" width="24.7109375" customWidth="1"/>
     <col min="15" max="15" width="22.28515625" customWidth="1"/>
     <col min="16" max="16" width="14.5703125" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:19">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1" t="s">
+      <c r="M2" s="3"/>
+      <c r="N2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="8"/>
     </row>
-    <row r="3" spans="2:18">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+    <row r="3" spans="2:19">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="2" t="s">
+      <c r="K3" s="3"/>
+      <c r="L3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="2" t="s">
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="R3" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="S3" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" spans="2:18">
-      <c r="I4" s="3"/>
+    <row r="4" spans="2:19">
+      <c r="I4" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:R2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -593,6 +646,7 @@
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:M2"/>
+    <mergeCell ref="P2:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>